<commit_message>
Changes Has been made in Test Classes
</commit_message>
<xml_diff>
--- a/DataFolder/TestDataOfNaukri.com.xlsx
+++ b/DataFolder/TestDataOfNaukri.com.xlsx
@@ -22,10 +22,10 @@
     <t>Raju1992@@</t>
   </si>
   <si>
-    <t>rajumsuryawanshi17@gmail.com</t>
+    <t>rajemsuryawanshi17@gmail.com</t>
   </si>
   <si>
-    <t>rajemsuryawanshi17@gmail.com</t>
+    <t>rajumsuryawanshi19@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -403,7 +403,7 @@
     </row>
     <row r="4" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
@@ -413,7 +413,7 @@
     </row>
     <row r="7" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>